<commit_message>
Feature: Add PDF page links, built-in PDF preview, and auto A/C lookup in Streamlit app
</commit_message>
<xml_diff>
--- a/Master/AC_Master.xlsx
+++ b/Master/AC_Master.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\ocr\ocr_fin_cashflow\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\ocr\ocr_fin_cashflow\Master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{217AFB4E-9E67-4568-97A1-723A5D0F5C88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0397C1C-C5DC-4B86-B6D6-8812AA3FFA94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="3135" windowWidth="21600" windowHeight="11175" xr2:uid="{A7F38960-24A1-4788-AAD0-F62DDE823EB5}"/>
+    <workbookView xWindow="2250" yWindow="2250" windowWidth="21600" windowHeight="11175" xr2:uid="{A7F38960-24A1-4788-AAD0-F62DDE823EB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>ACNO</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>BANGKOK</t>
+  </si>
+  <si>
+    <t>Currency</t>
   </si>
 </sst>
 </file>
@@ -121,7 +124,11 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -132,6 +139,21 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{75E51A9A-D19D-4F0A-931F-55F9BDDAEFC9}" name="Table1" displayName="Table1" ref="A1:F4" totalsRowShown="0">
+  <autoFilter ref="A1:F4" xr:uid="{75E51A9A-D19D-4F0A-931F-55F9BDDAEFC9}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{520D8D52-1E69-4281-A309-3AF709AD9347}" name="ACNO" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{0E37C959-ED27-47A5-BA93-53729C42229A}" name="BankName"/>
+    <tableColumn id="3" xr3:uid="{D7C08144-4C1A-4C55-81A8-C0D3CDDE8CEE}" name="Branch"/>
+    <tableColumn id="4" xr3:uid="{34794D88-AE34-4880-86EA-1B5A4AEDBD6F}" name="AccountName"/>
+    <tableColumn id="5" xr3:uid="{2AC0367F-9DC5-49A0-BEDA-140AE58C6999}" name="AccountType"/>
+    <tableColumn id="6" xr3:uid="{771857C7-8054-4788-8560-11EE6C8CFF05}" name="Currency"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -451,19 +473,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99202081-D0FC-4696-ADB6-A9CDFB4852ED}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.375" customWidth="1"/>
     <col min="3" max="3" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.25" customWidth="1"/>
+    <col min="5" max="5" width="14.25" customWidth="1"/>
+    <col min="6" max="6" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -479,8 +505,11 @@
       <c r="E1" t="s">
         <v>8</v>
       </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -497,7 +526,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -514,7 +543,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -533,5 +562,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix: Robust OCR extraction and stable PDF preview logic
</commit_message>
<xml_diff>
--- a/Master/AC_Master.xlsx
+++ b/Master/AC_Master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\ocr\ocr_fin_cashflow\Master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0397C1C-C5DC-4B86-B6D6-8812AA3FFA94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{638756E4-D588-47B2-800B-84CD7B2F634F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="2250" windowWidth="21600" windowHeight="11175" xr2:uid="{A7F38960-24A1-4788-AAD0-F62DDE823EB5}"/>
+    <workbookView xWindow="6075" yWindow="6315" windowWidth="21600" windowHeight="11175" xr2:uid="{A7F38960-24A1-4788-AAD0-F62DDE823EB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="25">
   <si>
     <t>ACNO</t>
   </si>
@@ -71,9 +71,6 @@
     <t>Fix</t>
   </si>
   <si>
-    <t>'9943-000613-100</t>
-  </si>
-  <si>
     <t>800000066583</t>
   </si>
   <si>
@@ -81,6 +78,39 @@
   </si>
   <si>
     <t>Currency</t>
+  </si>
+  <si>
+    <t>9943-000613-100</t>
+  </si>
+  <si>
+    <t>9943-000613-002</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>CIMB</t>
+  </si>
+  <si>
+    <t>2200027067340</t>
+  </si>
+  <si>
+    <t>2000501927</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>2000971203</t>
+  </si>
+  <si>
+    <t>CNH</t>
+  </si>
+  <si>
+    <t>840-101-0018-164202-001</t>
+  </si>
+  <si>
+    <t>BBL -BKK (FCD)</t>
   </si>
 </sst>
 </file>
@@ -142,8 +172,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{75E51A9A-D19D-4F0A-931F-55F9BDDAEFC9}" name="Table1" displayName="Table1" ref="A1:F4" totalsRowShown="0">
-  <autoFilter ref="A1:F4" xr:uid="{75E51A9A-D19D-4F0A-931F-55F9BDDAEFC9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{75E51A9A-D19D-4F0A-931F-55F9BDDAEFC9}" name="Table1" displayName="Table1" ref="A1:F9" totalsRowShown="0">
+  <autoFilter ref="A1:F9" xr:uid="{75E51A9A-D19D-4F0A-931F-55F9BDDAEFC9}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{520D8D52-1E69-4281-A309-3AF709AD9347}" name="ACNO" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{0E37C959-ED27-47A5-BA93-53729C42229A}" name="BankName"/>
@@ -473,16 +503,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99202081-D0FC-4696-ADB6-A9CDFB4852ED}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.375" customWidth="1"/>
+    <col min="1" max="1" width="24.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.25" customWidth="1"/>
     <col min="5" max="5" width="14.25" customWidth="1"/>
@@ -506,7 +536,7 @@
         <v>8</v>
       </c>
       <c r="F1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
@@ -525,10 +555,13 @@
       <c r="E2" t="s">
         <v>9</v>
       </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -542,22 +575,128 @@
       <c r="E3" t="s">
         <v>10</v>
       </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Santander Parser and update chunk splitting logic
</commit_message>
<xml_diff>
--- a/Master/AC_Master.xlsx
+++ b/Master/AC_Master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\ocr\ocr_fin_cashflow\Master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75086C98-1135-4E67-B8F6-488E74C0CF69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CCDA1E9-A016-40C1-B055-D49B30A67B3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A7F38960-24A1-4788-AAD0-F62DDE823EB5}"/>
+    <workbookView xWindow="10782" yWindow="3195" windowWidth="22810" windowHeight="14230" xr2:uid="{A7F38960-24A1-4788-AAD0-F62DDE823EB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="30">
   <si>
     <t>ACNO</t>
   </si>
@@ -120,20 +120,31 @@
   </si>
   <si>
     <t>(BK)</t>
+  </si>
+  <si>
+    <t>0069-100128-251</t>
+  </si>
+  <si>
+    <t>Santander</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <charset val="222"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -144,7 +155,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -152,13 +163,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -181,8 +210,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{75E51A9A-D19D-4F0A-931F-55F9BDDAEFC9}" name="Table1" displayName="Table1" ref="A1:G9" totalsRowShown="0">
-  <autoFilter ref="A1:G9" xr:uid="{75E51A9A-D19D-4F0A-931F-55F9BDDAEFC9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{75E51A9A-D19D-4F0A-931F-55F9BDDAEFC9}" name="Table1" displayName="Table1" ref="A1:G10" totalsRowShown="0">
+  <autoFilter ref="A1:G10" xr:uid="{75E51A9A-D19D-4F0A-931F-55F9BDDAEFC9}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{520D8D52-1E69-4281-A309-3AF709AD9347}" name="ACNO" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{0E37C959-ED27-47A5-BA93-53729C42229A}" name="BankName"/>
@@ -513,22 +542,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99202081-D0FC-4696-ADB6-A9CDFB4852ED}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.95" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.19921875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.75" customWidth="1"/>
-    <col min="5" max="5" width="15.25" customWidth="1"/>
-    <col min="6" max="6" width="14.25" customWidth="1"/>
+    <col min="3" max="3" width="10.69921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.69921875" customWidth="1"/>
+    <col min="5" max="5" width="15.19921875" customWidth="1"/>
+    <col min="6" max="6" width="14.19921875" customWidth="1"/>
     <col min="7" max="7" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -551,7 +582,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -574,7 +605,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -597,7 +628,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -620,7 +651,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -643,7 +674,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -666,7 +697,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
@@ -689,7 +720,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -712,7 +743,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
@@ -732,6 +763,29 @@
         <v>9</v>
       </c>
       <c r="G9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="18.149999999999999" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>